<commit_message>
add new test xml, test class and update the excel data driven file
</commit_message>
<xml_diff>
--- a/ParaBank-AutomationSuite/testdata/registerdata.xlsx
+++ b/ParaBank-AutomationSuite/testdata/registerdata.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\eclipse-workspace\Java\ParaBank-AutomationSuite\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\ParaBank-AutomationSuite\ParaBank-AutomationSuite\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3C5BB2-5E44-4F2F-A0F5-B2912793999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F793EE2-5169-4BF3-8172-EF2573546D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" activeTab="4" xr2:uid="{77E24629-30B1-4693-814A-8C3195B09ECD}"/>
+    <workbookView xWindow="0" yWindow="1455" windowWidth="8970" windowHeight="7785" firstSheet="1" activeTab="4" xr2:uid="{77E24629-30B1-4693-814A-8C3195B09ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="registerDataTest" sheetId="1" r:id="rId1"/>
     <sheet name="validateMandatoryFields" sheetId="2" r:id="rId2"/>
     <sheet name="loginData" sheetId="3" r:id="rId3"/>
     <sheet name="negativeTransferTest" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="billPageDataTest" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>First Name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Payee Name</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -139,13 +136,28 @@
     <t>From Acount</t>
   </si>
   <si>
-    <t>Jeff</t>
-  </si>
-  <si>
-    <t>lagos</t>
-  </si>
-  <si>
-    <t>Lagos</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Iyara Ijumu LGA Kogi State</t>
+  </si>
+  <si>
+    <t>Kabba</t>
+  </si>
+  <si>
+    <t>Kogi</t>
+  </si>
+  <si>
+    <t>49292</t>
+  </si>
+  <si>
+    <t>09188282828</t>
+  </si>
+  <si>
+    <t>20004</t>
+  </si>
+  <si>
+    <t>Alemidan Ojo</t>
   </si>
 </sst>
 </file>
@@ -856,18 +868,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5645A513-5F4E-479A-92E0-2B2D662A3178}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -882,39 +902,51 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
       </c>
       <c r="I1" t="s">
         <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2">
-        <v>484894</v>
-      </c>
-      <c r="F2">
-        <v>819895893</v>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the register data excel file
</commit_message>
<xml_diff>
--- a/ParaBank-AutomationSuite/testdata/registerdata.xlsx
+++ b/ParaBank-AutomationSuite/testdata/registerdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\ParaBank-AutomationSuite\ParaBank-AutomationSuite\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F793EE2-5169-4BF3-8172-EF2573546D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA347D94-CB6E-4CE4-88E2-8EFEDB0E638C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1455" windowWidth="8970" windowHeight="7785" firstSheet="1" activeTab="4" xr2:uid="{77E24629-30B1-4693-814A-8C3195B09ECD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{77E24629-30B1-4693-814A-8C3195B09ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="registerDataTest" sheetId="1" r:id="rId1"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94764595-DA0A-482C-91AD-B96408B6D5AB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5645A513-5F4E-479A-92E0-2B2D662A3178}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>